<commit_message>
fix problem with missing calibrations in selection. replace resource mock file. clean code of old  files that were not being used
</commit_message>
<xml_diff>
--- a/resource_mock/data/2018B-2019A Telescope Schedules.xlsx
+++ b/resource_mock/data/2018B-2019A Telescope Schedules.xlsx
@@ -5133,6 +5133,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
+    <col customWidth="1" min="2" max="2" width="20.57"/>
     <col customWidth="1" min="3" max="3" width="6.86"/>
   </cols>
   <sheetData>
@@ -9377,8 +9378,8 @@
       <c r="B186" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D186" s="2" t="s">
-        <v>39</v>
+      <c r="D186" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="E186" s="2" t="s">
         <v>11</v>
@@ -9400,8 +9401,8 @@
       <c r="B187" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D187" s="2" t="s">
-        <v>39</v>
+      <c r="D187" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="E187" s="2" t="s">
         <v>11</v>

</xml_diff>